<commit_message>
Repair And Fixing Repo
</commit_message>
<xml_diff>
--- a/Lib_Repo_Excel/FileExcel_Digisales/SCD0321 - Data Front Liner.xlsx
+++ b/Lib_Repo_Excel/FileExcel_Digisales/SCD0321 - Data Front Liner.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1442\Desktop\DigiSales\Lib_Repo_Excel\FileExcel_Digisales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9C16B5D-CFEE-4757-9FE8-0804B7AA2C5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AED4104-BFB4-4374-B8D2-F07AB1FFB8BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3030" yWindow="3030" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SCD0321" sheetId="2" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
   <si>
     <t>SIDEBAR_SUBMENU_SUBMENU</t>
   </si>
@@ -140,10 +140,13 @@
     <t>Berhasil melakuakn syncrnz &amp; data sesuai</t>
   </si>
   <si>
-    <t>SELECT * FROM DigisalesNew..Tbl_Master_Role WHERE Id=1005 SELECT * FROM DigisalesNew..Tbl_Pegawai WHERE Role_Id=1005</t>
-  </si>
-  <si>
     <t>Melakukan melakuakn syncrnz dan data sesuai</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT * FROM DigisalesNew..Tbl_Master_Role WHERE Id=1005 </t>
+  </si>
+  <si>
+    <t>SELECT * FROM DigisalesNew..Tbl_Pegawai WHERE Role_Id=1005</t>
   </si>
 </sst>
 </file>
@@ -552,8 +555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0EAF5E5-8229-45B3-AC11-8AED029F52F4}">
   <dimension ref="A1:AB7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -577,7 +580,7 @@
     <col min="18" max="18" width="15.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="90.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="7.85546875" style="1" customWidth="1"/>
     <col min="23" max="23" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="24" max="25" width="15.42578125" style="1" customWidth="1"/>
@@ -699,14 +702,18 @@
       <c r="R2" s="9"/>
       <c r="S2" s="9"/>
       <c r="T2" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="U2" s="5"/>
+        <v>36</v>
+      </c>
+      <c r="U2" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="V2" s="5"/>
       <c r="W2" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="X2" s="10"/>
+        <v>35</v>
+      </c>
+      <c r="X2" s="10" t="s">
+        <v>35</v>
+      </c>
       <c r="Y2" s="10"/>
       <c r="Z2" s="7" t="s">
         <v>24</v>

</xml_diff>